<commit_message>
Updated with new nylon screws
Need input from Joseph
Need to update fire retardant bag
</commit_message>
<xml_diff>
--- a/PartsList/PartsList.xlsx
+++ b/PartsList/PartsList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="141">
   <si>
     <t>Part Description</t>
   </si>
@@ -652,10 +652,22 @@
     <t>IMU</t>
   </si>
   <si>
-    <t>4-40 X 1/2 Pan Head Phillips Machine Screw Nylon</t>
-  </si>
-  <si>
-    <t>406-440-12-7A21</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>2-56 X 3/8”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> Pan HEAD SLOTTED MACHINE SCREW NYLON</t>
+    </r>
   </si>
   <si>
     <t>PCB</t>
@@ -713,12 +725,6 @@
   </si>
   <si>
     <t>280-440-2</t>
-  </si>
-  <si>
-    <t>#4 AN FLAT WASHER, Nylon</t>
-  </si>
-  <si>
-    <t>302-40-7-FW4-093</t>
   </si>
   <si>
     <t>M3 X 18 0.5 PITCH METRIC SOCKET HEAD CAP SCREW 12.9 ALLOY STEEL DIN 912</t>
@@ -1991,14 +1997,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28.3281" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="64.8125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.9297" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.8516" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.4844" style="1" customWidth="1"/>
@@ -2796,7 +2802,9 @@
       <c r="A38" t="s" s="8">
         <v>105</v>
       </c>
-      <c r="B38" s="5"/>
+      <c r="B38" t="s" s="9">
+        <v>106</v>
+      </c>
       <c r="C38" s="6"/>
       <c r="D38" t="s" s="8">
         <v>106</v>
@@ -2926,16 +2934,14 @@
         <v>122</v>
       </c>
       <c r="B44" s="9"/>
-      <c r="C44" t="s" s="2">
-        <v>123</v>
-      </c>
+      <c r="C44" s="15"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="10">
         <v>4</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -2944,11 +2950,11 @@
     </row>
     <row r="45" ht="19" customHeight="1">
       <c r="A45" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" t="s" s="16">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -2956,7 +2962,7 @@
         <v>10</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -2965,11 +2971,11 @@
     </row>
     <row r="46" ht="19" customHeight="1">
       <c r="A46" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" t="s" s="16">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -2977,7 +2983,7 @@
         <v>18</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
@@ -2986,11 +2992,11 @@
     </row>
     <row r="47" ht="19" customHeight="1">
       <c r="A47" t="s" s="2">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" t="s" s="16">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -2998,7 +3004,7 @@
         <v>8</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -3007,11 +3013,11 @@
     </row>
     <row r="48" ht="19" customHeight="1">
       <c r="A48" t="s" s="2">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" t="s" s="16">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -3026,11 +3032,11 @@
     </row>
     <row r="49" ht="19" customHeight="1">
       <c r="A49" t="s" s="2">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" t="s" s="16">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -3045,16 +3051,16 @@
     </row>
     <row r="50" ht="19" customHeight="1">
       <c r="A50" t="s" s="2">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B50" s="5"/>
-      <c r="C50" t="s" s="16">
-        <v>139</v>
+      <c r="C50" s="17">
+        <v>15417</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
@@ -3064,16 +3070,16 @@
     </row>
     <row r="51" ht="19" customHeight="1">
       <c r="A51" t="s" s="2">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="17">
-        <v>15417</v>
+        <v>16866</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
@@ -3083,11 +3089,11 @@
     </row>
     <row r="52" ht="19" customHeight="1">
       <c r="A52" t="s" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="17">
-        <v>16866</v>
+        <v>16864</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -3100,19 +3106,13 @@
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="53" ht="19" customHeight="1">
-      <c r="A53" t="s" s="2">
-        <v>142</v>
-      </c>
+    <row r="53" ht="17" customHeight="1">
+      <c r="A53" s="15"/>
       <c r="B53" s="5"/>
-      <c r="C53" s="17">
-        <v>16864</v>
-      </c>
+      <c r="C53" s="6"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
-      <c r="F53" s="10">
-        <v>8</v>
-      </c>
+      <c r="F53" s="4"/>
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
@@ -3139,11 +3139,13 @@
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
+      <c r="G55" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
     </row>
     <row r="56" ht="17" customHeight="1">
       <c r="A56" s="15"/>
@@ -3152,13 +3154,11 @@
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
     </row>
     <row r="57" ht="17" customHeight="1">
       <c r="A57" s="15"/>
@@ -3237,19 +3237,6 @@
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
       <c r="K62" s="15"/>
-    </row>
-    <row r="63" ht="17" customHeight="1">
-      <c r="A63" s="15"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="15"/>
-      <c r="K63" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>